<commit_message>
adding notes about formulas
</commit_message>
<xml_diff>
--- a/week2-Metrics for Measuring Brand Assets/Formulas for Calculations Demonstrated in this Module.xlsx
+++ b/week2-Metrics for Measuring Brand Assets/Formulas for Calculations Demonstrated in this Module.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Brand equity = (Revenue Premium - Additional Variable cost) * Long-term multiplier</t>
   </si>
@@ -50,9 +50,6 @@
     <t>LTM = (1 + d) / (1 + d - r)</t>
   </si>
   <si>
-    <t>d= discount rate r = stability factor Long-term multiplier discounts the value of brand equity to its net present value.</t>
-  </si>
-  <si>
     <t>Purpose</t>
   </si>
   <si>
@@ -63,6 +60,16 @@
   </si>
   <si>
     <t>To use revenue premium as a measure of brand equity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>price is Private Label's price
+UniteSale is Brand's Unite sales</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d= discount rate 
+r = stability factor Long-term multiplier discounts the value of brand equity to its net present value.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -70,7 +77,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +88,14 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
@@ -130,7 +145,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -138,6 +153,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -423,7 +441,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -435,18 +453,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -471,9 +489,11 @@
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="57" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -481,11 +501,12 @@
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>